<commit_message>
Final proposal and Gantt
</commit_message>
<xml_diff>
--- a/Documents/FInal Presentation/Gantt.xlsx
+++ b/Documents/FInal Presentation/Gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8BEF3-952C-4F84-AFB2-2466162DD646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6D61F-ECC4-4071-8942-36DA4A5E23FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Project Planner</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1076,7 @@
   <dimension ref="B1:AQ30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1153,7 +1150,7 @@
       </c>
       <c r="H2" s="15">
         <f ca="1">IF(YEAR(TODAY())=2024, WEEKNUM(TODAY())-36, WEEKNUM(TODAY())+16)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="34" t="s">
@@ -1461,20 +1458,20 @@
       <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>43</v>
+      <c r="C8" s="7">
+        <v>5</v>
       </c>
       <c r="D8" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G8" s="8">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1482,16 +1479,16 @@
         <v>34</v>
       </c>
       <c r="C9" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E9" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G9" s="8">
         <v>0.2</v>
@@ -1502,13 +1499,13 @@
         <v>39</v>
       </c>
       <c r="C10" s="7">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F10" s="7">
         <v>1</v>
@@ -1522,19 +1519,19 @@
         <v>35</v>
       </c>
       <c r="C11" s="7">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11" s="7">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E11" s="7">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1542,19 +1539,19 @@
         <v>38</v>
       </c>
       <c r="C12" s="7">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E12" s="7">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F12" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on final presentation
</commit_message>
<xml_diff>
--- a/Documents/FInal Presentation/Gantt.xlsx
+++ b/Documents/FInal Presentation/Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6D61F-ECC4-4071-8942-36DA4A5E23FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC6375-2F0C-418A-95BA-1629C201FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t>Project Planner</t>
-  </si>
-  <si>
     <t>ACTIVITY</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>Rocket Flight Computer</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1076,7 @@
   <dimension ref="B1:AQ30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1093,7 +1093,7 @@
   <sheetData>
     <row r="1" spans="2:43" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1139,22 +1139,22 @@
     </row>
     <row r="2" spans="2:43" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="15">
         <f ca="1">IF(YEAR(TODAY())=2024, WEEKNUM(TODAY())-36, WEEKNUM(TODAY())+16)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
@@ -1162,21 +1162,21 @@
       <c r="O2" s="36"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R2" s="37"/>
       <c r="S2" s="37"/>
       <c r="T2" s="36"/>
       <c r="U2" s="18"/>
       <c r="V2" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W2" s="28"/>
       <c r="X2" s="28"/>
       <c r="Y2" s="38"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB2" s="28"/>
       <c r="AC2" s="28"/>
@@ -1186,7 +1186,7 @@
       <c r="AG2" s="38"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AJ2" s="28"/>
       <c r="AK2" s="28"/>
@@ -1198,25 +1198,25 @@
     </row>
     <row r="3" spans="2:43" s="12" customFormat="1" ht="39.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="E3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="F3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="G3" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>26</v>
-      </c>
       <c r="H3" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
@@ -1228,13 +1228,13 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W3" s="39"/>
       <c r="X3" s="39"/>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="5" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="6" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7">
         <v>2</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="7" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="8" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="7">
         <v>5</v>
@@ -1468,15 +1468,15 @@
         <v>5</v>
       </c>
       <c r="F8" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7">
         <v>8</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="10" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7">
         <v>10</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="11" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="7">
         <v>9</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="12" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="7">
         <v>8</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="13" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>15</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="14" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7">
         <v>33</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="15" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="16" spans="2:43" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="9">
         <v>0</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="9">
         <v>0</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="9">
         <v>0</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="9">
         <v>0</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" s="9">
         <v>0</v>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="9">
         <v>0</v>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="7">
         <v>0</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="9">
         <v>0</v>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="7">
         <v>0</v>

</xml_diff>